<commit_message>
wrote clusring results work on document
</commit_message>
<xml_diff>
--- a/data/index_time.xlsx
+++ b/data/index_time.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="19155" windowHeight="8505"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="19155" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Index 100 docs" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Querying time" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>Time in secs</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>h</t>
+  </si>
+  <si>
+    <t>length</t>
   </si>
 </sst>
 </file>
@@ -150,6 +153,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -166,7 +237,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="D6D6D6"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -447,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,15 +807,15 @@
         <v>12</v>
       </c>
       <c r="B23">
-        <f>B22/60</f>
+        <f t="shared" ref="B23:D24" si="1">B22/60</f>
         <v>2754</v>
       </c>
       <c r="C23">
-        <f>C22/60</f>
+        <f t="shared" si="1"/>
         <v>2546</v>
       </c>
       <c r="D23">
-        <f>D22/60</f>
+        <f t="shared" si="1"/>
         <v>1768</v>
       </c>
     </row>
@@ -753,15 +824,15 @@
         <v>13</v>
       </c>
       <c r="B24">
-        <f>B23/60</f>
+        <f t="shared" si="1"/>
         <v>45.9</v>
       </c>
       <c r="C24">
-        <f>C23/60</f>
+        <f t="shared" si="1"/>
         <v>42.43333333333333</v>
       </c>
       <c r="D24">
-        <f>D23/60</f>
+        <f t="shared" si="1"/>
         <v>29.466666666666665</v>
       </c>
     </row>
@@ -773,12 +844,222 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="D1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>70</v>
+      </c>
+      <c r="E2">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="F2">
+        <v>0.38800000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>70</v>
+      </c>
+      <c r="E3">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="F3">
+        <v>0.30499999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>70</v>
+      </c>
+      <c r="E4">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="F4">
+        <v>0.28799999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <f>AVERAGE(E2:E4)</f>
+        <v>0.17800000000000002</v>
+      </c>
+      <c r="F5">
+        <f>AVERAGE(F2:F4)</f>
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="G5">
+        <f>F5/E5</f>
+        <v>1.8370786516853932</v>
+      </c>
+    </row>
+    <row r="6" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>198</v>
+      </c>
+      <c r="E6">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="F6">
+        <v>0.72799999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>198</v>
+      </c>
+      <c r="E7">
+        <v>0.15</v>
+      </c>
+      <c r="F7">
+        <v>0.89500000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>198</v>
+      </c>
+      <c r="E8">
+        <v>0.221</v>
+      </c>
+      <c r="F8">
+        <v>0.80900000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <f>AVERAGE(E6:E8)</f>
+        <v>0.17900000000000002</v>
+      </c>
+      <c r="F9">
+        <f>AVERAGE(F6:F8)</f>
+        <v>0.81066666666666665</v>
+      </c>
+      <c r="G9">
+        <f>F9/E9</f>
+        <v>4.5288640595903162</v>
+      </c>
+    </row>
+    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>452</v>
+      </c>
+      <c r="E10">
+        <v>0.307</v>
+      </c>
+      <c r="F10">
+        <v>2.4969999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>452</v>
+      </c>
+      <c r="E11">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="F11">
+        <v>1.2849999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>452</v>
+      </c>
+      <c r="E12">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="F12">
+        <v>1.2949999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <f>AVERAGE(E10:E12)</f>
+        <v>0.32333333333333331</v>
+      </c>
+      <c r="F13">
+        <f>AVERAGE(F10:F12)</f>
+        <v>1.6923333333333332</v>
+      </c>
+      <c r="G13">
+        <f>F13/E13</f>
+        <v>5.2340206185567011</v>
+      </c>
+    </row>
+    <row r="14" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>771</v>
+      </c>
+      <c r="E14">
+        <v>0.372</v>
+      </c>
+      <c r="F14">
+        <v>2.2589999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>771</v>
+      </c>
+      <c r="E15">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="F15">
+        <v>1.921</v>
+      </c>
+    </row>
+    <row r="16" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>771</v>
+      </c>
+      <c r="E16">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="F16">
+        <v>2.0190000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <f>AVERAGE(E14:E16)</f>
+        <v>0.39333333333333337</v>
+      </c>
+      <c r="F17">
+        <f>AVERAGE(F14:F16)</f>
+        <v>2.0663333333333331</v>
+      </c>
+      <c r="G17">
+        <f>F17/E17</f>
+        <v>5.2533898305084739</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>